<commit_message>
Switch sim to package
Former-commit-id: 7da95a5e822faf93a6776f6880618c5fb974f1bc
</commit_message>
<xml_diff>
--- a/simulationTesting/simulation-arguments.xlsx
+++ b/simulationTesting/simulation-arguments.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="31080" yWindow="3540" windowWidth="30240" windowHeight="17260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,16 +44,16 @@
     <t>base</t>
   </si>
   <si>
-    <t>cv_obs</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
     <t>case</t>
   </si>
   <si>
-    <t>sigma_t</t>
+    <t>gp_sigma</t>
+  </si>
+  <si>
+    <t>sd_obs</t>
   </si>
 </sst>
 </file>
@@ -108,8 +108,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -218,7 +222,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -270,6 +274,8 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -321,6 +327,8 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -599,7 +607,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -618,16 +626,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -641,7 +649,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>0.2</v>
@@ -667,7 +675,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>0.2</v>
@@ -693,7 +701,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>0.2</v>
@@ -719,7 +727,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>0.2</v>
@@ -745,7 +753,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>0.2</v>
@@ -771,7 +779,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>0.2</v>
@@ -797,7 +805,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>0.2</v>
@@ -823,7 +831,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <v>0.2</v>
@@ -849,7 +857,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>0.2</v>
@@ -875,7 +883,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <v>0.2</v>
@@ -901,7 +909,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>0.2</v>
@@ -927,7 +935,7 @@
         <v>20</v>
       </c>
       <c r="D13" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E13">
         <v>0.2</v>
@@ -953,7 +961,7 @@
         <v>30</v>
       </c>
       <c r="D14" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E14">
         <v>0.2</v>
@@ -979,7 +987,7 @@
         <v>15</v>
       </c>
       <c r="D15" s="1">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="E15">
         <v>0.2</v>
@@ -991,7 +999,7 @@
         <v>3</v>
       </c>
       <c r="H15">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1005,7 +1013,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>0.2</v>
@@ -1017,7 +1025,7 @@
         <v>3</v>
       </c>
       <c r="H16">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1031,7 +1039,7 @@
         <v>15</v>
       </c>
       <c r="D17" s="1">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="E17">
         <v>0.2</v>
@@ -1043,7 +1051,7 @@
         <v>3</v>
       </c>
       <c r="H17">
-        <v>0.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1057,7 +1065,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E18">
         <v>0.2</v>
@@ -1069,7 +1077,7 @@
         <v>3</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1083,7 +1091,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E19" s="1">
         <v>0.05</v>
@@ -1092,7 +1100,7 @@
         <v>0.5</v>
       </c>
       <c r="G19" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H19">
         <v>0.05</v>
@@ -1109,7 +1117,7 @@
         <v>15</v>
       </c>
       <c r="D20" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E20" s="1">
         <v>0.1</v>
@@ -1118,7 +1126,7 @@
         <v>0.5</v>
       </c>
       <c r="G20" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H20">
         <v>0.1</v>
@@ -1135,7 +1143,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E21" s="1">
         <v>0.4</v>
@@ -1144,7 +1152,7 @@
         <v>0.5</v>
       </c>
       <c r="G21" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H21">
         <v>0.4</v>
@@ -1161,7 +1169,7 @@
         <v>15</v>
       </c>
       <c r="D22" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E22" s="1">
         <v>0.8</v>
@@ -1170,7 +1178,7 @@
         <v>0.5</v>
       </c>
       <c r="G22" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H22">
         <v>0.8</v>
@@ -1187,7 +1195,7 @@
         <v>15</v>
       </c>
       <c r="D23" s="2">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E23" s="1">
         <v>1.2</v>
@@ -1196,7 +1204,7 @@
         <v>0.5</v>
       </c>
       <c r="G23" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H23">
         <v>1.2</v>

</xml_diff>